<commit_message>
Cambios generales en Informes de avance
Actualizado el formato del xls y del doc
</commit_message>
<xml_diff>
--- a/Entregables/Informe de avance/Informe de avance.xlsx
+++ b/Entregables/Informe de avance/Informe de avance.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Actualización del plan de proyecto. </t>
   </si>
   <si>
-    <t>Actualización del plan de proyecto. Creación de los ambientes de trabajo. Creación documentos de roles,</t>
+    <t>Actualización del plan de proyecto. Creación de los ambientes de trabajo. Creación documentos de Roles; Habilidades y Competencias; Riesgos; Comunicación; WBS.</t>
   </si>
 </sst>
 </file>
@@ -76,7 +76,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -101,14 +101,14 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -116,10 +116,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -127,26 +140,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,156 +465,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K13"/>
+  <dimension ref="B3:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:K10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="6" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="6" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="9">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6">
         <v>42110</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="9">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6">
         <v>42117</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="9">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
         <v>42124</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="9">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6">
         <v>42130</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C13:K13"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="C10:K10"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="C10:M10"/>
+    <mergeCell ref="C11:M11"/>
+    <mergeCell ref="C12:M12"/>
+    <mergeCell ref="C13:M13"/>
+    <mergeCell ref="C9:M9"/>
+    <mergeCell ref="C8:M8"/>
+    <mergeCell ref="C7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>